<commit_message>
code and data update
</commit_message>
<xml_diff>
--- a/Data/Antechinus_data.xlsx
+++ b/Data/Antechinus_data.xlsx
@@ -2149,7 +2149,7 @@
   <dimension ref="A1:Q188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2740,7 +2740,7 @@
         <v>25</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>69</v>
@@ -2846,7 +2846,7 @@
         <v>25</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>69</v>
@@ -2899,7 +2899,7 @@
         <v>25</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>69</v>
@@ -2952,7 +2952,7 @@
         <v>25</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
data update (cleaned specimens chunk)
</commit_message>
<xml_diff>
--- a/Data/Antechinus_data.xlsx
+++ b/Data/Antechinus_data.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="577">
   <si>
     <t>Species</t>
   </si>
@@ -2151,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2169,7 +2169,7 @@
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="107.21875" bestFit="1" customWidth="1"/>
@@ -4112,7 +4112,7 @@
         <v>25</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>69</v>
@@ -4165,10 +4165,10 @@
         <v>25</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>69</v>
+        <v>576</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>69</v>
+        <v>576</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>69</v>
@@ -4218,7 +4218,7 @@
         <v>25</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>69</v>
@@ -4271,7 +4271,7 @@
         <v>25</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>69</v>
@@ -4324,7 +4324,7 @@
         <v>25</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>69</v>
@@ -4430,7 +4430,7 @@
         <v>25</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O43" s="1" t="s">
         <v>69</v>
@@ -4483,7 +4483,7 @@
         <v>25</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O44" s="1" t="s">
         <v>69</v>
@@ -4536,7 +4536,7 @@
         <v>25</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>69</v>
@@ -4589,7 +4589,7 @@
         <v>25</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>69</v>
@@ -4642,7 +4642,7 @@
         <v>25</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O47" s="1" t="s">
         <v>69</v>
@@ -4695,7 +4695,7 @@
         <v>25</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>69</v>
@@ -4748,7 +4748,7 @@
         <v>25</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O49" s="1" t="s">
         <v>69</v>
@@ -4801,7 +4801,7 @@
         <v>25</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O50" s="1" t="s">
         <v>69</v>
@@ -4854,7 +4854,7 @@
         <v>25</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>69</v>
@@ -4907,7 +4907,7 @@
         <v>25</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>69</v>
@@ -4960,7 +4960,7 @@
         <v>25</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>69</v>
@@ -5013,7 +5013,7 @@
         <v>25</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>69</v>
@@ -5066,7 +5066,7 @@
         <v>25</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>69</v>
@@ -5119,7 +5119,7 @@
         <v>25</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O56" s="1" t="s">
         <v>69</v>
@@ -5172,7 +5172,7 @@
         <v>25</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O57" s="1" t="s">
         <v>69</v>
@@ -5225,7 +5225,7 @@
         <v>25</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O58" s="1" t="s">
         <v>69</v>
@@ -5278,7 +5278,7 @@
         <v>25</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O59" s="1" t="s">
         <v>69</v>
@@ -5331,7 +5331,7 @@
         <v>25</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
data update (chunk of cleaned specimens)
</commit_message>
<xml_diff>
--- a/Data/Antechinus_data.xlsx
+++ b/Data/Antechinus_data.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="577">
   <si>
     <t>Species</t>
   </si>
@@ -1850,7 +1850,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Antechinus_data" displayName="Antechinus_data" ref="A1:Q188" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:Q188"/>
+  <autoFilter ref="A1:Q188">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="ok"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="17">
     <tableColumn id="35" uniqueName="35" name="Species" queryTableFieldId="1"/>
     <tableColumn id="36" uniqueName="36" name="Collection" queryTableFieldId="2"/>
@@ -2151,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2169,7 +2175,7 @@
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.21875" customWidth="1"/>
     <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="107.21875" bestFit="1" customWidth="1"/>
@@ -4124,7 +4130,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -5384,7 +5390,7 @@
         <v>25</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O61" s="1" t="s">
         <v>69</v>
@@ -5490,7 +5496,7 @@
         <v>25</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O63" s="1" t="s">
         <v>69</v>
@@ -5543,7 +5549,7 @@
         <v>25</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O64" s="1" t="s">
         <v>69</v>
@@ -5596,7 +5602,7 @@
         <v>25</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O65" s="1" t="s">
         <v>69</v>
@@ -5649,7 +5655,7 @@
         <v>25</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O66" s="1" t="s">
         <v>69</v>
@@ -5702,7 +5708,7 @@
         <v>25</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O67" s="1" t="s">
         <v>69</v>
@@ -5755,7 +5761,7 @@
         <v>25</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O68" s="1" t="s">
         <v>69</v>
@@ -5808,7 +5814,7 @@
         <v>25</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O69" s="1" t="s">
         <v>69</v>
@@ -5861,7 +5867,7 @@
         <v>25</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>69</v>
@@ -5914,7 +5920,7 @@
         <v>25</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>69</v>
@@ -6020,7 +6026,7 @@
         <v>25</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O73" s="1" t="s">
         <v>69</v>
@@ -6073,7 +6079,7 @@
         <v>25</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O74" s="1" t="s">
         <v>69</v>
@@ -6179,7 +6185,7 @@
         <v>25</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O76" s="1" t="s">
         <v>69</v>
@@ -6232,7 +6238,7 @@
         <v>25</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O77" s="1" t="s">
         <v>69</v>
@@ -6285,7 +6291,7 @@
         <v>25</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O78" s="1" t="s">
         <v>69</v>
@@ -6338,7 +6344,7 @@
         <v>25</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O79" s="1" t="s">
         <v>69</v>
@@ -6391,7 +6397,7 @@
         <v>25</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O80" s="1" t="s">
         <v>69</v>
@@ -6444,7 +6450,7 @@
         <v>25</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O81" s="1" t="s">
         <v>69</v>
@@ -6456,7 +6462,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>29</v>
       </c>
@@ -6497,7 +6503,7 @@
         <v>25</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>25</v>
+        <v>576</v>
       </c>
       <c r="O82" s="1" t="s">
         <v>576</v>
@@ -6550,7 +6556,7 @@
         <v>25</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O83" s="1" t="s">
         <v>69</v>
@@ -6603,7 +6609,7 @@
         <v>25</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O84" s="1" t="s">
         <v>69</v>
@@ -6656,7 +6662,7 @@
         <v>25</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O85" s="1" t="s">
         <v>69</v>
@@ -6709,7 +6715,7 @@
         <v>25</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O86" s="1" t="s">
         <v>69</v>
@@ -6762,7 +6768,7 @@
         <v>25</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O87" s="1" t="s">
         <v>69</v>
@@ -6815,7 +6821,7 @@
         <v>25</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O88" s="1" t="s">
         <v>69</v>
@@ -6868,7 +6874,7 @@
         <v>25</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O89" s="1" t="s">
         <v>69</v>
@@ -6921,7 +6927,7 @@
         <v>25</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O90" s="1" t="s">
         <v>69</v>
@@ -6974,7 +6980,7 @@
         <v>25</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O91" s="1" t="s">
         <v>69</v>
@@ -7080,7 +7086,7 @@
         <v>25</v>
       </c>
       <c r="N93" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O93" s="1" t="s">
         <v>69</v>
@@ -7133,7 +7139,7 @@
         <v>25</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O94" s="1" t="s">
         <v>69</v>
@@ -7186,7 +7192,7 @@
         <v>25</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O95" s="1" t="s">
         <v>69</v>
@@ -7239,7 +7245,7 @@
         <v>25</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O96" s="1" t="s">
         <v>69</v>
@@ -7292,7 +7298,7 @@
         <v>25</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O97" s="1" t="s">
         <v>69</v>
@@ -7345,7 +7351,7 @@
         <v>25</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O98" s="1" t="s">
         <v>69</v>
@@ -7398,7 +7404,7 @@
         <v>25</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O99" s="1" t="s">
         <v>69</v>
@@ -7451,7 +7457,7 @@
         <v>25</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O100" s="1" t="s">
         <v>69</v>
@@ -7504,7 +7510,7 @@
         <v>25</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O101" s="1" t="s">
         <v>69</v>
@@ -7610,7 +7616,7 @@
         <v>25</v>
       </c>
       <c r="N103" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O103" s="1" t="s">
         <v>69</v>
@@ -7663,7 +7669,7 @@
         <v>25</v>
       </c>
       <c r="N104" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O104" s="1" t="s">
         <v>69</v>
@@ -7716,7 +7722,7 @@
         <v>25</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O105" s="1" t="s">
         <v>69</v>
@@ -7769,7 +7775,7 @@
         <v>25</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O106" s="1" t="s">
         <v>69</v>
@@ -7822,7 +7828,7 @@
         <v>25</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O107" s="1" t="s">
         <v>69</v>
@@ -7875,7 +7881,7 @@
         <v>25</v>
       </c>
       <c r="N108" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O108" s="1" t="s">
         <v>69</v>
@@ -7928,7 +7934,7 @@
         <v>25</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O109" s="1" t="s">
         <v>69</v>
@@ -7981,7 +7987,7 @@
         <v>25</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O110" s="1" t="s">
         <v>69</v>
@@ -8034,7 +8040,7 @@
         <v>25</v>
       </c>
       <c r="N111" s="1" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="O111" s="1" t="s">
         <v>69</v>
@@ -8099,7 +8105,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>29</v>
       </c>
@@ -8152,7 +8158,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>17</v>
       </c>
@@ -8205,7 +8211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>17</v>
       </c>
@@ -8258,7 +8264,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>17</v>
       </c>
@@ -8311,7 +8317,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>17</v>
       </c>
@@ -8364,7 +8370,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>17</v>
       </c>
@@ -8417,7 +8423,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>17</v>
       </c>
@@ -8470,7 +8476,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>29</v>
       </c>
@@ -8523,7 +8529,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>17</v>
       </c>
@@ -8629,7 +8635,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>17</v>
       </c>
@@ -8682,7 +8688,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>17</v>
       </c>
@@ -8735,7 +8741,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>17</v>
       </c>
@@ -8788,7 +8794,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>17</v>
       </c>
@@ -8841,7 +8847,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>17</v>
       </c>
@@ -8894,7 +8900,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>17</v>
       </c>
@@ -8947,7 +8953,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>29</v>
       </c>
@@ -9000,7 +9006,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>29</v>
       </c>
@@ -9053,7 +9059,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>17</v>
       </c>
@@ -9159,7 +9165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>29</v>
       </c>
@@ -9212,7 +9218,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>17</v>
       </c>
@@ -9265,7 +9271,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>29</v>
       </c>
@@ -9318,7 +9324,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>29</v>
       </c>
@@ -9371,7 +9377,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>29</v>
       </c>
@@ -9477,7 +9483,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>29</v>
       </c>
@@ -9530,7 +9536,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>29</v>
       </c>
@@ -9583,7 +9589,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>29</v>
       </c>
@@ -9689,7 +9695,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>17</v>
       </c>
@@ -9742,7 +9748,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>17</v>
       </c>
@@ -9789,7 +9795,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>17</v>
       </c>
@@ -9842,7 +9848,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>29</v>
       </c>
@@ -9895,7 +9901,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>17</v>
       </c>
@@ -9948,7 +9954,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>17</v>
       </c>
@@ -10001,7 +10007,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>17</v>
       </c>
@@ -10054,7 +10060,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>17</v>
       </c>
@@ -10107,7 +10113,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>17</v>
       </c>
@@ -10213,7 +10219,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>17</v>
       </c>
@@ -10266,7 +10272,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>17</v>
       </c>
@@ -10319,7 +10325,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>17</v>
       </c>
@@ -10372,7 +10378,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>17</v>
       </c>
@@ -10425,7 +10431,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>17</v>
       </c>
@@ -10478,7 +10484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>17</v>
       </c>
@@ -10531,7 +10537,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>29</v>
       </c>
@@ -10584,7 +10590,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>29</v>
       </c>
@@ -10637,7 +10643,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>29</v>
       </c>
@@ -10743,7 +10749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>29</v>
       </c>
@@ -10796,7 +10802,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>29</v>
       </c>
@@ -10849,7 +10855,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>29</v>
       </c>
@@ -10902,7 +10908,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>17</v>
       </c>
@@ -10955,7 +10961,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>17</v>
       </c>
@@ -11008,7 +11014,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>17</v>
       </c>
@@ -11061,7 +11067,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>29</v>
       </c>
@@ -11114,7 +11120,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>29</v>
       </c>
@@ -11167,7 +11173,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>17</v>
       </c>
@@ -11273,7 +11279,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>29</v>
       </c>
@@ -11326,7 +11332,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>29</v>
       </c>
@@ -11379,7 +11385,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>29</v>
       </c>
@@ -11432,7 +11438,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>29</v>
       </c>
@@ -11485,7 +11491,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>29</v>
       </c>
@@ -11538,7 +11544,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>29</v>
       </c>
@@ -11591,7 +11597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>29</v>
       </c>
@@ -11644,7 +11650,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>29</v>
       </c>
@@ -11697,7 +11703,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>29</v>
       </c>
@@ -11803,7 +11809,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>17</v>
       </c>
@@ -11856,7 +11862,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>29</v>
       </c>
@@ -11909,7 +11915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>29</v>
       </c>
@@ -11962,7 +11968,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>29</v>
       </c>
@@ -12015,7 +12021,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>17</v>
       </c>
@@ -12068,7 +12074,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
population data update, figure update and code update
</commit_message>
<xml_diff>
--- a/Data/Antechinus_data.xlsx
+++ b/Data/Antechinus_data.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Antechinus_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Antechinus_data!$H$1:$H$181</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Antechinus_data!$B$1:$B$181</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="463">
   <si>
     <t>Species</t>
   </si>
@@ -1410,10 +1410,7 @@
     <t>qm or bust - dunno about this one - but you could guestimate based on description</t>
   </si>
   <si>
-    <t>subtropicus holotype</t>
-  </si>
-  <si>
-    <t>stuartii neotype</t>
+    <t>exclude? Sub?</t>
   </si>
 </sst>
 </file>
@@ -2223,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,6 +2230,7 @@
     <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="81.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
@@ -3564,7 +3562,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -3617,7 +3615,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
         <v>39</v>
@@ -3835,7 +3833,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>463</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
         <v>405</v>
@@ -5093,7 +5091,7 @@
         <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C53" t="s">
         <v>405</v>
@@ -5152,7 +5150,7 @@
         <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C54" t="s">
         <v>405</v>
@@ -5208,7 +5206,7 @@
         <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
         <v>20</v>
@@ -5373,7 +5371,7 @@
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
         <v>405</v>
@@ -5485,7 +5483,7 @@
         <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>
@@ -5541,7 +5539,7 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C61" t="s">
         <v>405</v>
@@ -5586,7 +5584,7 @@
         <v>26</v>
       </c>
       <c r="Q61" t="s">
-        <v>185</v>
+        <v>31</v>
       </c>
       <c r="R61" t="s">
         <v>36</v>
@@ -7451,7 +7449,7 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>462</v>
+        <v>19</v>
       </c>
       <c r="C95" t="s">
         <v>20</v>
@@ -7625,7 +7623,7 @@
         <v>19</v>
       </c>
       <c r="B98" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C98" t="s">
         <v>20</v>
@@ -8141,7 +8139,7 @@
         <v>30</v>
       </c>
       <c r="B107" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C107" t="s">
         <v>20</v>
@@ -8516,7 +8514,7 @@
         <v>26</v>
       </c>
       <c r="Q113" t="s">
-        <v>138</v>
+        <v>462</v>
       </c>
       <c r="R113" t="s">
         <v>36</v>
@@ -11499,7 +11497,7 @@
         <v>30</v>
       </c>
       <c r="B169" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C169" t="s">
         <v>20</v>
@@ -12208,7 +12206,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H181"/>
+  <autoFilter ref="B1:B181"/>
   <sortState ref="A2:S181">
     <sortCondition ref="H157"/>
   </sortState>

</xml_diff>

<commit_message>
code update (addition of seasonality)
</commit_message>
<xml_diff>
--- a/Data/Antechinus_data.xlsx
+++ b/Data/Antechinus_data.xlsx
@@ -2284,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:XFD104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2300,13 +2300,13 @@
     <col min="8" max="8" width="81.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5546875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="11" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="107.21875" bestFit="1" customWidth="1"/>

</xml_diff>